<commit_message>
excel makes no sense
</commit_message>
<xml_diff>
--- a/multitable.xlsx
+++ b/multitable.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wb1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="wb2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -50,6 +51,24 @@
   </si>
   <si>
     <t xml:space="preserve">Hello World</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// For whatever reason the first date is in MM/DD/YY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23/07/1976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// So is this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/01/2038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// This is a string</t>
   </si>
 </sst>
 </file>
@@ -127,7 +146,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,6 +157,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -159,8 +182,8 @@
   </sheetPr>
   <dimension ref="B3:AC18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -260,6 +283,23 @@
         <v>26.74</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -270,4 +310,69 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="n">
+        <v>43586</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="n">
+        <v>31595</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>